<commit_message>
time and activate result of exam and score board
</commit_message>
<xml_diff>
--- a/class_1_participant.xlsx
+++ b/class_1_participant.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,16 +462,7 @@
           <t>حسنی</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>09100069381</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0025109391</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -489,37 +480,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>09120912011</t>
+          <t>02938423984</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0200184776</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>محسن</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>حسنی</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>093284902384</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0923847238</t>
+          <t>0239482309</t>
         </is>
       </c>
     </row>

</xml_diff>